<commit_message>
added worksheet 'Updated_labels_parents' documented changes made in the ontologies, refs #37048
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@99283 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/plasmodium_labels.xlsx
+++ b/Load/ontology/harmonization/plasmodium_labels.xlsx
@@ -5,27 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/ontology/eupath/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F399F-5025-C04B-8A89-21851DF5040D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AF02C2-50AB-C749-9401-C439FF22B5FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="460" windowWidth="28740" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="detection_template_csv" sheetId="1" r:id="rId1"/>
-    <sheet name="antibiotics" sheetId="3" r:id="rId2"/>
-    <sheet name="lookup" sheetId="2" r:id="rId3"/>
+    <sheet name="Updated_labels_parents" sheetId="4" r:id="rId1"/>
+    <sheet name="detection_template_csv" sheetId="1" r:id="rId2"/>
+    <sheet name="antibiotics" sheetId="3" r:id="rId3"/>
+    <sheet name="lookup" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">detection_template_csv!$A$1:$Q$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">detection_template_csv!$A$1:$Q$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Updated_labels_parents!$A$1:$F$71</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="216">
   <si>
     <t>variable</t>
   </si>
@@ -568,6 +570,111 @@
   </si>
   <si>
     <t>categorical</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by thin smear microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium in blood</t>
+  </si>
+  <si>
+    <t>Eukaryota in blood</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by Ministry of Health microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by Lima quality control lab qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium, by thick smear microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium, by RDT</t>
+  </si>
+  <si>
+    <t>Plasmodium, by thin smear microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages, by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes, by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stage density categorization, by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium, by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium density categorization, by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium species, by control lab microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium, by multiple methods</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax gametocytes (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax Ct value, by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum asexual stages (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum (copies per rxn), by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum Ct value, by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax asexual stages (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium falciparum gametocytes (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium vivax (copies per rxn), by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium gametocytes (per 500 WBC), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages (per 500 WBC), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium asexual stages (per uL blood), by microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium (per uL), by qPCR</t>
+  </si>
+  <si>
+    <t>Plasmodium (per 100 WBC), by thick smear microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium (per 200 WBC), by thick smear microscopy</t>
+  </si>
+  <si>
+    <t>Plasmodium (per 500 RBC), by thin smear microscopy</t>
+  </si>
+  <si>
+    <t>Denominator, by thick smear microscopy</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1170,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1078,6 +1185,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1432,12 +1542,1459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A236212D-BBB7-9F42-AAE2-B353EEF8535E}">
+  <dimension ref="A1:F71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="68.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F71" xr:uid="{78625AC4-5C29-2941-967E-68D0F0D647C8}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,7 +3844,7 @@
         <v>('data item' and is about some Plasmodium species) and is_specified_output_of some (('Ministry of Health microscopy assay' and achieves_planned_objective some 'organism identification objective') and has_specified_input some 'blood specimen from organism')</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -5205,7 +6762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0DB369-D91D-804D-8D4A-F6F9B2BC7AF1}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -5241,7 +6798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AA4B01-1A62-8B4E-8367-99824A1C2D4E}">
   <dimension ref="A1:D4"/>
   <sheetViews>

</xml_diff>